<commit_message>
predictions updated using weather data
</commit_message>
<xml_diff>
--- a/future_prediction/usa/Weekly-Deaths-Prediction r = 1.xlsx
+++ b/future_prediction/usa/Weekly-Deaths-Prediction r = 1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="63">
   <si>
     <t>the day the prediction is made</t>
   </si>
@@ -560,7 +560,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K48"/>
+  <dimension ref="A1:K49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1598,6 +1598,32 @@
         <v>24.59</v>
       </c>
     </row>
+    <row r="49" spans="1:11">
+      <c r="A49" t="s">
+        <v>14</v>
+      </c>
+      <c r="B49" t="s">
+        <v>61</v>
+      </c>
+      <c r="C49">
+        <v>3333.57</v>
+      </c>
+      <c r="D49">
+        <v>2251.19</v>
+      </c>
+      <c r="E49">
+        <v>1082.38</v>
+      </c>
+      <c r="F49" t="s">
+        <v>62</v>
+      </c>
+      <c r="J49">
+        <v>823.1</v>
+      </c>
+      <c r="K49">
+        <v>26.17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>